<commit_message>
Updated Script for figures
Add code files for making figures.
Commented new definition of g_PMCA.  Added 2 new parameters in SS file - p(42) & p(43)
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/642b98f60231af7b/Desktop/Research _Rangamani/SkelMuscleCa-main/SkelMuscleCa_Git_ank012/Parameter Estimation/PSO_1_26/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/642b98f60231af7b/Documents/GitHub/SkelMuscleCa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:1_{206615E0-3786-46E1-B87C-31FD196CCE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4993396-4E75-4CB2-9464-36EFAC37A6F9}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{206615E0-3786-46E1-B87C-31FD196CCE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BB01A17-5238-40E1-8170-13CB27C9C7B1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
+    <workbookView xWindow="3810" yWindow="1875" windowWidth="28800" windowHeight="15345" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>A_a</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>K_mK_NKX</t>
+  </si>
+  <si>
+    <t>nu_SERCA</t>
+  </si>
+  <si>
+    <t>g_PMCA</t>
   </si>
 </sst>
 </file>
@@ -213,14 +219,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -258,7 +260,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -364,7 +366,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -506,7 +508,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -514,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,6 +861,22 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>4875</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>5.37</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E1:F41">
     <sortCondition ref="E1:E41"/>

</xml_diff>

<commit_message>
Update input parameter list to include SERCA, PMCA, and SR leak. Lower values for SERCA, PMCA, SR leak, and NCX flux in the lb/ub range for fitting (and in the sweep file). Set Kd for CSQN to 800 as discussed.
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/642b98f60231af7b/Documents/GitHub/SkelMuscleCa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucsdcloud-my.sharepoint.com/personal/eafrancis_ucsd_edu/Documents/Documents/Rangamani Lab/MATLAB/Muscle calcium model/SkelMuscleCa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="105" documentId="13_ncr:1_{206615E0-3786-46E1-B87C-31FD196CCE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BB01A17-5238-40E1-8170-13CB27C9C7B1}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="13_ncr:1_{206615E0-3786-46E1-B87C-31FD196CCE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{413581AD-B4C7-436A-ABC9-0240D373125F}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="1875" windowWidth="28800" windowHeight="15345" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="16590" windowHeight="14580" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>A_a</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>g_PMCA</t>
+  </si>
+  <si>
+    <t>nu_leakSR</t>
   </si>
 </sst>
 </file>
@@ -516,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,6 +880,14 @@
         <v>5.37</v>
       </c>
     </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>0.2</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E1:F41">
     <sortCondition ref="E1:E41"/>

</xml_diff>

<commit_message>
Fig 4 code updates
Updated the code for function plotting figures, and added code for plotting fig 4
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{206615E0-3786-46E1-B87C-31FD196CCE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AD8C2E8-F5A2-4705-B4D8-830E58175E9A}"/>
   <bookViews>
-    <workbookView xWindow="13335" yWindow="2775" windowWidth="28800" windowHeight="15345" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
+    <workbookView xWindow="7380" yWindow="2520" windowWidth="28800" windowHeight="15345" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -220,10 +220,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -525,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
   <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update ranges used for fitting parameters, return vector of currents, add back sweep script.
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/642b98f60231af7b/Documents/GitHub/SkelMuscleCa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucsdcloud-my.sharepoint.com/personal/eafrancis_ucsd_edu/Documents/Documents/Rangamani Lab/MATLAB/Muscle calcium model/SkelMuscleCa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{206615E0-3786-46E1-B87C-31FD196CCE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AD8C2E8-F5A2-4705-B4D8-830E58175E9A}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="13_ncr:1_{206615E0-3786-46E1-B87C-31FD196CCE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7542EB58-EDB7-430A-AEA7-08807F34729B}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="2520" windowWidth="28800" windowHeight="15345" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
+    <workbookView xWindow="21810" yWindow="735" windowWidth="16590" windowHeight="14580" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>A_a</t>
   </si>
@@ -164,10 +164,13 @@
     <t>nu_SERCA</t>
   </si>
   <si>
+    <t>g_PMCA</t>
+  </si>
+  <si>
     <t>nu_leakSR</t>
   </si>
   <si>
-    <t>g_PMCA</t>
+    <t>g_leakNa</t>
   </si>
 </sst>
 </file>
@@ -220,6 +223,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -519,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,7 +884,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>0.2</v>
+        <v>5.37</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -885,7 +892,15 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>5.37</v>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>2E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Error in loading the xlsxfile
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/642b98f60231af7b/Documents/GitHub/SkelMuscleCa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucsdcloud-my.sharepoint.com/personal/eafrancis_ucsd_edu/Documents/Documents/Rangamani Lab/MATLAB/Muscle calcium model/SkelMuscleCa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="13_ncr:1_{206615E0-3786-46E1-B87C-31FD196CCE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AD8C2E8-F5A2-4705-B4D8-830E58175E9A}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="13_ncr:1_{206615E0-3786-46E1-B87C-31FD196CCE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7542EB58-EDB7-430A-AEA7-08807F34729B}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="2520" windowWidth="28800" windowHeight="15345" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
+    <workbookView xWindow="21810" yWindow="735" windowWidth="16590" windowHeight="14580" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>A_a</t>
   </si>
@@ -164,10 +164,13 @@
     <t>nu_SERCA</t>
   </si>
   <si>
+    <t>g_PMCA</t>
+  </si>
+  <si>
     <t>nu_leakSR</t>
   </si>
   <si>
-    <t>g_PMCA</t>
+    <t>g_leakNa</t>
   </si>
 </sst>
 </file>
@@ -220,6 +223,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -519,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,7 +884,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>0.2</v>
+        <v>5.37</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -885,7 +892,15 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>5.37</v>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>2E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scripts for diff exercises
Updated the list of expt in dydt, and added scripts for computing dynamics for diff exercises.
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucsdcloud-my.sharepoint.com/personal/eafrancis_ucsd_edu/Documents/Documents/Rangamani Lab/MATLAB/Muscle calcium model/SkelMuscleCa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/642b98f60231af7b/Documents/GitHub/SkelMuscleCa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="13_ncr:1_{206615E0-3786-46E1-B87C-31FD196CCE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7542EB58-EDB7-430A-AEA7-08807F34729B}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{206615E0-3786-46E1-B87C-31FD196CCE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCE1A4FD-4136-494F-B0FC-D5B6A84BE368}"/>
   <bookViews>
-    <workbookView xWindow="21810" yWindow="735" windowWidth="16590" windowHeight="14580" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -223,10 +224,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -528,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changed phosphate conc to uM instead of mM ; tried to update parameters and PP "if" statements; now using mass action instead of if statements ... (maybe)
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/642b98f60231af7b/Documents/GitHub/SkelMuscleCa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juliette\Documents\MATLAB\SkelMuscle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{9A2AE787-EF16-4A03-8A4E-826D38F6E0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE5CEB3D-124D-42B0-B60F-365F801FE877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
+    <workbookView xWindow="15180" yWindow="0" windowWidth="13740" windowHeight="15585" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>A_a</t>
   </si>
@@ -172,6 +171,96 @@
   </si>
   <si>
     <t>g_leakNa</t>
+  </si>
+  <si>
+    <t>k_onMA</t>
+  </si>
+  <si>
+    <t>k_offMA</t>
+  </si>
+  <si>
+    <t>kHYD</t>
+  </si>
+  <si>
+    <t>kH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_on0 </t>
+  </si>
+  <si>
+    <t>k_off0</t>
+  </si>
+  <si>
+    <t>k_onCa</t>
+  </si>
+  <si>
+    <t>k_offCa</t>
+  </si>
+  <si>
+    <t>f0</t>
+  </si>
+  <si>
+    <t>h0</t>
+  </si>
+  <si>
+    <t>hP</t>
+  </si>
+  <si>
+    <t>g0</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>kP</t>
+  </si>
+  <si>
+    <t>Ap</t>
+  </si>
+  <si>
+    <t>Bp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bP </t>
+  </si>
+  <si>
+    <t>k_onATP</t>
+  </si>
+  <si>
+    <t>k_offATP</t>
+  </si>
+  <si>
+    <t>k_onParvCa</t>
+  </si>
+  <si>
+    <t>k_offParvCa</t>
+  </si>
+  <si>
+    <t>k_onParvMg</t>
+  </si>
+  <si>
+    <t>k_offParvMg</t>
+  </si>
+  <si>
+    <t>Parv_itot</t>
+  </si>
+  <si>
+    <t>k_onTrop</t>
+  </si>
+  <si>
+    <t>k_offTrop</t>
+  </si>
+  <si>
+    <t>Mg</t>
+  </si>
+  <si>
+    <t>fP</t>
+  </si>
+  <si>
+    <t>kPROD</t>
+  </si>
+  <si>
+    <t>Trop_tot</t>
   </si>
 </sst>
 </file>
@@ -212,10 +301,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -231,10 +320,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -534,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,590 +638,697 @@
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1">
         <v>150</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="4"/>
+      <c r="E1" s="3"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>7.5</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="4"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>5.8</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>8.1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>288</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>13.1</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="4"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>100</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>4380</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>1380</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>67</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11">
         <v>0.01</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12">
         <v>500</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13">
         <v>-25000</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="4"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14">
         <v>0.4</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15">
         <v>0.2</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="4"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16">
         <v>0.1</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="4"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17">
         <v>0.64800000000000002</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="3"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18">
         <v>0.111</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="3"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19">
         <v>8.0399999999999991</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="4"/>
+      <c r="E19" s="3"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20">
         <v>0.129</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="4"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21">
         <v>3.5420000000000003E-5</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="E21" s="3"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22">
         <v>14.7</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="3"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23">
         <v>10</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="3"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24">
         <v>7</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="4"/>
+      <c r="E24" s="3"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25">
         <v>9</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="4"/>
+      <c r="E25" s="3"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26">
         <v>18</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="4"/>
+      <c r="E26" s="3"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27">
         <v>40</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="4"/>
+      <c r="E27" s="3"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28">
         <v>950000000</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="E28" s="3"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29">
         <v>1000</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="4"/>
+      <c r="E29" s="3"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30">
         <v>13000</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="4"/>
+      <c r="E30" s="3"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31">
         <v>0.17</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="4"/>
+      <c r="E31" s="3"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32">
         <v>4.5</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="4"/>
+      <c r="E32" s="3"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33">
         <v>1000000</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="4"/>
+      <c r="E33" s="3"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34">
         <v>1</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="4"/>
+      <c r="E34" s="3"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35">
         <v>1</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="4"/>
+      <c r="E35" s="3"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36">
         <v>0.05</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="4"/>
+      <c r="E36" s="3"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>32</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37">
         <v>6.59</v>
       </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="4"/>
+      <c r="E37" s="3"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38">
         <v>0.32</v>
       </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="4"/>
+      <c r="E38" s="3"/>
       <c r="F38" s="1"/>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>34</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39">
         <v>0.27</v>
       </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="4"/>
+      <c r="E39" s="3"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40">
         <v>10000</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="4"/>
+      <c r="E40" s="3"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41">
         <v>0.01</v>
       </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42">
         <v>4875</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="4"/>
+      <c r="E42" s="3"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43">
         <v>5.37</v>
       </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="4"/>
+      <c r="E43" s="3"/>
       <c r="F43" s="1"/>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44">
         <v>0.2</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="4"/>
+      <c r="E44" s="3"/>
       <c r="F44" s="1"/>
-      <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45">
         <v>2E-3</v>
       </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="2"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48">
+        <v>41.7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>67</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="4">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>46</v>
+      </c>
+      <c r="B54">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>73</v>
+      </c>
+      <c r="B57">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>69</v>
+      </c>
+      <c r="B59">
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>49</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>50</v>
+      </c>
+      <c r="B62">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>51</v>
+      </c>
+      <c r="B63">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>52</v>
+      </c>
+      <c r="B64">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>53</v>
+      </c>
+      <c r="B65">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>54</v>
+      </c>
+      <c r="B67">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>55</v>
+      </c>
+      <c r="B68">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>56</v>
+      </c>
+      <c r="B69">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>57</v>
+      </c>
+      <c r="B70">
+        <v>6000000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>58</v>
+      </c>
+      <c r="B71">
+        <v>8.3799999999999999E-2</v>
+      </c>
+      <c r="C71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>59</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>60</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>61</v>
+      </c>
+      <c r="B74">
+        <v>2.8670000000000001E-2</v>
+      </c>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>140</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E1:G37">
@@ -1145,4 +1337,254 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001C39BCF8C10C0F4DBE17E99B61C93E7A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3b5ed46e2a2a5b06309d3f0a93e8cdba">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xmlns:ns4="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24ef5abf4ddcd47874225b9eda8b4566" ns3:_="" ns4:_="">
+    <xsd:import namespace="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
+    <xsd:import namespace="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:_activity" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_activity" ma:index="13" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="14" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="15" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="12" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7950FF80-637C-480D-8472-1E87FBE72C09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
+    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05EA78B-E099-49AE-BE0F-B2667B8D5E8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FACC7053-B3AF-4F0E-A33A-4CFF5AC23007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added new parameters, trying to fix phosphate equations
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juliette\Documents\MATLAB\SkelMuscle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE5CEB3D-124D-42B0-B60F-365F801FE877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{63E68CC2-1CB3-491E-AC37-3EAB7901EBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="0" windowWidth="13740" windowHeight="15585" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
+    <workbookView xWindow="15060" yWindow="165" windowWidth="13740" windowHeight="13020" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>A_a</t>
   </si>
@@ -261,6 +261,12 @@
   </si>
   <si>
     <t>Trop_tot</t>
+  </si>
+  <si>
+    <t>p_i_SR_init</t>
+  </si>
+  <si>
+    <t>Pi_Myo_init</t>
   </si>
 </sst>
 </file>
@@ -299,12 +305,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,10 +1142,10 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+      <c r="A52" t="s">
         <v>68</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B52">
         <v>1500</v>
       </c>
     </row>
@@ -1328,6 +1333,22 @@
       </c>
       <c r="B75">
         <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>3000</v>
       </c>
     </row>
   </sheetData>
@@ -1340,6 +1361,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001C39BCF8C10C0F4DBE17E99B61C93E7A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3b5ed46e2a2a5b06309d3f0a93e8cdba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xmlns:ns4="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24ef5abf4ddcd47874225b9eda8b4566" ns3:_="" ns4:_="">
     <xsd:import namespace="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
@@ -1528,24 +1566,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FACC7053-B3AF-4F0E-A33A-4CFF5AC23007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05EA78B-E099-49AE-BE0F-B2667B8D5E8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7950FF80-637C-480D-8472-1E87FBE72C09}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1562,29 +1608,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05EA78B-E099-49AE-BE0F-B2667B8D5E8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FACC7053-B3AF-4F0E-A33A-4CFF5AC23007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ran second sensitivity analysis (5-10.mat), updated test run code
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juliette\Documents\MATLAB\SkelMuscle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63E68CC2-1CB3-491E-AC37-3EAB7901EBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0C49245-67DF-4F66-B38B-56A5C0CE4114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15060" yWindow="165" windowWidth="13740" windowHeight="13020" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
+    <workbookView xWindow="15060" yWindow="165" windowWidth="13740" windowHeight="14925" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -273,8 +273,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="177" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -305,11 +306,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,7 +1108,7 @@
         <v>63</v>
       </c>
       <c r="B47">
-        <v>30000</v>
+        <v>300</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1117,7 +1119,7 @@
         <v>41.7</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>65</v>
       </c>
@@ -1125,7 +1127,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>66</v>
       </c>
@@ -1133,7 +1135,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>67</v>
       </c>
@@ -1141,7 +1143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>68</v>
       </c>
@@ -1149,7 +1151,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>45</v>
       </c>
@@ -1157,7 +1159,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -1165,7 +1167,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>47</v>
       </c>
@@ -1173,7 +1175,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -1181,7 +1183,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>73</v>
       </c>
@@ -1189,7 +1191,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>71</v>
       </c>
@@ -1197,7 +1199,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>69</v>
       </c>
@@ -1205,7 +1207,7 @@
         <v>88.5</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>70</v>
       </c>
@@ -1213,7 +1215,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>49</v>
       </c>
@@ -1221,7 +1223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>50</v>
       </c>
@@ -1229,15 +1231,16 @@
         <v>150</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>51</v>
       </c>
       <c r="B63">
         <v>150</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>52</v>
       </c>
@@ -1298,7 +1301,7 @@
         <v>58</v>
       </c>
       <c r="B71">
-        <v>8.3799999999999999E-2</v>
+        <v>3.62E-3</v>
       </c>
       <c r="C71" s="2"/>
     </row>
@@ -1307,7 +1310,7 @@
         <v>59</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1315,7 +1318,7 @@
         <v>60</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>9.9999999999999995E-8</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1325,7 +1328,7 @@
       <c r="B74">
         <v>2.8670000000000001E-2</v>
       </c>
-      <c r="D74" s="2"/>
+      <c r="D74" s="4"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">

</xml_diff>

<commit_message>
ran two PSOs, edited some of the files to adjust to new estimated parameters.
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juliette\Documents\MATLAB\SkelMuscle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0C49245-67DF-4F66-B38B-56A5C0CE4114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8111740C-A651-464C-AC48-8BEDEAE32637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15060" yWindow="165" windowWidth="13740" windowHeight="14925" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="177" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -311,7 +311,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="E80" sqref="E80"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +760,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="1"/>
@@ -1364,23 +1364,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001C39BCF8C10C0F4DBE17E99B61C93E7A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3b5ed46e2a2a5b06309d3f0a93e8cdba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xmlns:ns4="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24ef5abf4ddcd47874225b9eda8b4566" ns3:_="" ns4:_="">
     <xsd:import namespace="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
@@ -1569,32 +1552,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FACC7053-B3AF-4F0E-A33A-4CFF5AC23007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05EA78B-E099-49AE-BE0F-B2667B8D5E8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7950FF80-637C-480D-8472-1E87FBE72C09}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1611,4 +1586,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05EA78B-E099-49AE-BE0F-B2667B8D5E8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FACC7053-B3AF-4F0E-A33A-4CFF5AC23007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
more updates, trying to rerun original model and compare
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juliette\Documents\MATLAB\SkelMuscle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8111740C-A651-464C-AC48-8BEDEAE32637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9D2278-9E5A-43E5-8051-060C22B422C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>A_a</t>
   </si>
@@ -267,6 +267,57 @@
   </si>
   <si>
     <t>Pi_Myo_init</t>
+  </si>
+  <si>
+    <t>V_a</t>
+  </si>
+  <si>
+    <t>V_h</t>
+  </si>
+  <si>
+    <t>V_hkinf</t>
+  </si>
+  <si>
+    <t>V_m</t>
+  </si>
+  <si>
+    <t>V_n</t>
+  </si>
+  <si>
+    <t>V_Sinf</t>
+  </si>
+  <si>
+    <t>V_tau</t>
+  </si>
+  <si>
+    <t>VBar_RyR</t>
+  </si>
+  <si>
+    <t>kATP</t>
+  </si>
+  <si>
+    <t>KmNa_i_NCX</t>
+  </si>
+  <si>
+    <t>KmNa_EC_NCX</t>
+  </si>
+  <si>
+    <t>Kmc_EC_NCX_N</t>
+  </si>
+  <si>
+    <t>g_SLLeak</t>
+  </si>
+  <si>
+    <t>L_RyR</t>
+  </si>
+  <si>
+    <t>g0_DHPR</t>
+  </si>
+  <si>
+    <t>j0_RyR</t>
+  </si>
+  <si>
+    <t>Kmc_EC_NCX_C</t>
   </si>
 </sst>
 </file>
@@ -626,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,6 +1405,145 @@
         <v>3000</v>
       </c>
     </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>-46</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>-78</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>12290</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>87500</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>93</v>
+      </c>
+      <c r="B90">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>9.9999999999999991E-6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>9.3900000000000011E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>43846000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="2"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E1:G37">
     <sortCondition ref="E1:E37"/>
@@ -1364,6 +1554,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001C39BCF8C10C0F4DBE17E99B61C93E7A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3b5ed46e2a2a5b06309d3f0a93e8cdba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xmlns:ns4="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24ef5abf4ddcd47874225b9eda8b4566" ns3:_="" ns4:_="">
     <xsd:import namespace="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
@@ -1552,24 +1759,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FACC7053-B3AF-4F0E-A33A-4CFF5AC23007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05EA78B-E099-49AE-BE0F-B2667B8D5E8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7950FF80-637C-480D-8472-1E87FBE72C09}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1586,29 +1801,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05EA78B-E099-49AE-BE0F-B2667B8D5E8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FACC7053-B3AF-4F0E-A33A-4CFF5AC23007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
new updates, no more D0 and D1, now a six-state crossbridge model
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juliette\Documents\MATLAB\SkelMuscle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9D2278-9E5A-43E5-8051-060C22B422C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B699667-F80E-432E-9C1A-BE3C8AE29920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>A_a</t>
   </si>
@@ -245,12 +245,6 @@
     <t>Parv_itot</t>
   </si>
   <si>
-    <t>k_onTrop</t>
-  </si>
-  <si>
-    <t>k_offTrop</t>
-  </si>
-  <si>
     <t>Mg</t>
   </si>
   <si>
@@ -318,6 +312,18 @@
   </si>
   <si>
     <t>Kmc_EC_NCX_C</t>
+  </si>
+  <si>
+    <t>k_onTrop1</t>
+  </si>
+  <si>
+    <t>k_offTrop1</t>
+  </si>
+  <si>
+    <t>k_onTrop2</t>
+  </si>
+  <si>
+    <t>k_offTrop2</t>
   </si>
 </sst>
 </file>
@@ -679,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
   <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,7 +1157,7 @@
         <v>62</v>
       </c>
       <c r="B46">
-        <v>150</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1236,7 +1242,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B57">
         <v>100</v>
@@ -1244,7 +1250,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B58">
         <v>1000</v>
@@ -1252,18 +1258,18 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="B59">
-        <v>88.5</v>
+        <v>177</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="B60">
-        <v>115</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1309,7 +1315,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B66">
         <v>15000</v>
@@ -1383,7 +1389,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B75">
         <v>140</v>
@@ -1391,7 +1397,7 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B76">
         <v>3000</v>
@@ -1399,7 +1405,7 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B77">
         <v>3000</v>
@@ -1407,7 +1413,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B78">
         <v>70</v>
@@ -1415,7 +1421,7 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B79">
         <v>-45</v>
@@ -1423,7 +1429,7 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B80">
         <v>-40</v>
@@ -1431,7 +1437,7 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B81">
         <v>-46</v>
@@ -1439,7 +1445,7 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B82">
         <v>-40</v>
@@ -1447,7 +1453,7 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B83">
         <v>-78</v>
@@ -1455,7 +1461,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B84">
         <v>90</v>
@@ -1463,7 +1469,7 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B85">
         <v>-20</v>
@@ -1471,7 +1477,7 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B86">
         <v>0.04</v>
@@ -1479,7 +1485,7 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B87">
         <v>12290</v>
@@ -1487,7 +1493,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B88">
         <v>87500</v>
@@ -1495,7 +1501,7 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B89">
         <v>1300</v>
@@ -1503,7 +1509,7 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B90">
         <v>1600</v>
@@ -1511,7 +1517,7 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B91">
         <v>9.9999999999999991E-6</v>
@@ -1519,7 +1525,7 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B92">
         <v>500000</v>
@@ -1527,7 +1533,7 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B93">
         <v>9.3900000000000011E-2</v>
@@ -1535,13 +1541,27 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B94">
         <v>43846000</v>
       </c>
     </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>88.5</v>
+      </c>
+    </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>17.100000000000001</v>
+      </c>
       <c r="D96" s="2"/>
     </row>
   </sheetData>
@@ -1554,23 +1574,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001C39BCF8C10C0F4DBE17E99B61C93E7A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3b5ed46e2a2a5b06309d3f0a93e8cdba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xmlns:ns4="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24ef5abf4ddcd47874225b9eda8b4566" ns3:_="" ns4:_="">
     <xsd:import namespace="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
@@ -1759,7 +1762,43 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7950FF80-637C-480D-8472-1E87FBE72C09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
+    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FACC7053-B3AF-4F0E-A33A-4CFF5AC23007}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1776,29 +1815,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05EA78B-E099-49AE-BE0F-B2667B8D5E8C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7950FF80-637C-480D-8472-1E87FBE72C09}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
-    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
more updates, added ATP depence on D2
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juliette\Documents\MATLAB\SkelMuscle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B699667-F80E-432E-9C1A-BE3C8AE29920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CE5BDDC-4D0F-4724-BB78-40E82A0C9099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>A_a</t>
   </si>
@@ -183,12 +183,6 @@
   </si>
   <si>
     <t>kH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_on0 </t>
-  </si>
-  <si>
-    <t>k_off0</t>
   </si>
   <si>
     <t>k_onCa</t>
@@ -685,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
   <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:D21"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,7 +1148,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B46">
         <v>15</v>
@@ -1162,7 +1156,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B47">
         <v>300</v>
@@ -1170,7 +1164,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B48">
         <v>41.7</v>
@@ -1178,7 +1172,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B49">
         <v>0.5</v>
@@ -1186,7 +1180,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B50">
         <v>3.3000000000000002E-2</v>
@@ -1194,7 +1188,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B51">
         <v>3</v>
@@ -1202,7 +1196,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B52">
         <v>1500</v>
@@ -1242,7 +1236,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B57">
         <v>100</v>
@@ -1250,7 +1244,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B58">
         <v>1000</v>
@@ -1258,7 +1252,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B59">
         <v>177</v>
@@ -1266,7 +1260,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B60">
         <v>1544</v>
@@ -1277,7 +1271,7 @@
         <v>49</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1285,7 +1279,7 @@
         <v>50</v>
       </c>
       <c r="B62">
-        <v>150</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1293,32 +1287,32 @@
         <v>51</v>
       </c>
       <c r="B63">
-        <v>150</v>
+        <v>1500</v>
       </c>
       <c r="E63" s="2"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B64">
-        <v>50</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B65">
-        <v>1500</v>
+        <v>240</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B66">
-        <v>15000</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1326,7 +1320,7 @@
         <v>54</v>
       </c>
       <c r="B67">
-        <v>240</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1334,7 +1328,7 @@
         <v>55</v>
       </c>
       <c r="B68">
-        <v>180</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1342,7 +1336,7 @@
         <v>56</v>
       </c>
       <c r="B69">
-        <v>120</v>
+        <v>3.62E-3</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1350,7 +1344,7 @@
         <v>57</v>
       </c>
       <c r="B70">
-        <v>6000000</v>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1358,7 +1352,7 @@
         <v>58</v>
       </c>
       <c r="B71">
-        <v>3.62E-3</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="C71" s="2"/>
     </row>
@@ -1367,23 +1361,23 @@
         <v>59</v>
       </c>
       <c r="B72">
-        <v>9.9999999999999995E-7</v>
+        <v>2.8670000000000001E-2</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B73">
-        <v>9.9999999999999995E-8</v>
+        <v>140</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="B74">
-        <v>2.8670000000000001E-2</v>
+        <v>3000</v>
       </c>
       <c r="D74" s="4"/>
     </row>
@@ -1392,7 +1386,7 @@
         <v>72</v>
       </c>
       <c r="B75">
-        <v>140</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1400,7 +1394,7 @@
         <v>73</v>
       </c>
       <c r="B76">
-        <v>3000</v>
+        <v>70</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1408,7 +1402,7 @@
         <v>74</v>
       </c>
       <c r="B77">
-        <v>3000</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1416,7 +1410,7 @@
         <v>75</v>
       </c>
       <c r="B78">
-        <v>70</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1424,7 +1418,7 @@
         <v>76</v>
       </c>
       <c r="B79">
-        <v>-45</v>
+        <v>-46</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1440,7 +1434,7 @@
         <v>78</v>
       </c>
       <c r="B81">
-        <v>-46</v>
+        <v>-78</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -1448,7 +1442,7 @@
         <v>79</v>
       </c>
       <c r="B82">
-        <v>-40</v>
+        <v>90</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1456,7 +1450,7 @@
         <v>80</v>
       </c>
       <c r="B83">
-        <v>-78</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1464,7 +1458,7 @@
         <v>81</v>
       </c>
       <c r="B84">
-        <v>90</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -1472,7 +1466,7 @@
         <v>82</v>
       </c>
       <c r="B85">
-        <v>-20</v>
+        <v>12290</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1480,7 +1474,7 @@
         <v>83</v>
       </c>
       <c r="B86">
-        <v>0.04</v>
+        <v>87500</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1488,31 +1482,31 @@
         <v>84</v>
       </c>
       <c r="B87">
-        <v>12290</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B88">
-        <v>87500</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B89">
-        <v>1300</v>
+        <v>9.9999999999999991E-6</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B90">
-        <v>1600</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -1520,7 +1514,7 @@
         <v>87</v>
       </c>
       <c r="B91">
-        <v>9.9999999999999991E-6</v>
+        <v>9.3900000000000011E-2</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -1528,40 +1522,26 @@
         <v>88</v>
       </c>
       <c r="B92">
-        <v>500000</v>
+        <v>43846000</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B93">
-        <v>9.3900000000000011E-2</v>
+        <v>88.5</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B94">
-        <v>43846000</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>94</v>
-      </c>
-      <c r="B95">
-        <v>88.5</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>95</v>
-      </c>
-      <c r="B96">
-        <v>17.100000000000001</v>
-      </c>
       <c r="D96" s="2"/>
     </row>
   </sheetData>
@@ -1574,6 +1554,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001C39BCF8C10C0F4DBE17E99B61C93E7A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3b5ed46e2a2a5b06309d3f0a93e8cdba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xmlns:ns4="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24ef5abf4ddcd47874225b9eda8b4566" ns3:_="" ns4:_="">
     <xsd:import namespace="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
@@ -1762,14 +1750,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1780,6 +1760,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FACC7053-B3AF-4F0E-A33A-4CFF5AC23007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7950FF80-637C-480D-8472-1E87FBE72C09}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1798,23 +1795,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FACC7053-B3AF-4F0E-A33A-4CFF5AC23007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05EA78B-E099-49AE-BE0F-B2667B8D5E8C}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
created SkelMuscleObj function, tried to clean up some files as well
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juliette\Documents\MATLAB\SkelMuscle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CE5BDDC-4D0F-4724-BB78-40E82A0C9099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1B888C9-60CF-44EB-B952-F504D66BCA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>A_a</t>
   </si>
@@ -318,15 +318,19 @@
   </si>
   <si>
     <t>k_offTrop2</t>
+  </si>
+  <si>
+    <t>g_SOCE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="173" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -357,12 +361,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,16 +682,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
-  <dimension ref="A1:F96"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="G98" sqref="G98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -811,7 +816,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>300</v>
+        <v>0.25</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="1"/>
@@ -1541,8 +1546,19 @@
         <v>17.100000000000001</v>
       </c>
     </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+      <c r="B95" s="5">
+        <v>4.7519482988025094E-5</v>
+      </c>
+    </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D96" s="2"/>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B103" s="5"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E1:G37">
@@ -1562,6 +1578,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001C39BCF8C10C0F4DBE17E99B61C93E7A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3b5ed46e2a2a5b06309d3f0a93e8cdba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xmlns:ns4="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24ef5abf4ddcd47874225b9eda8b4566" ns3:_="" ns4:_="">
     <xsd:import namespace="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
@@ -1750,15 +1775,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FACC7053-B3AF-4F0E-A33A-4CFF5AC23007}">
   <ds:schemaRefs>
@@ -1777,6 +1793,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05EA78B-E099-49AE-BE0F-B2667B8D5E8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7950FF80-637C-480D-8472-1E87FBE72C09}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1793,12 +1817,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05EA78B-E099-49AE-BE0F-B2667B8D5E8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Introduce new compartments for junctional vs bulk spaces and add new parameters associated with diffusion between these new regions. Delete old files and clean up code, only one dydt function now.
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juliette\Documents\MATLAB\SkelMuscle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucsdcloud-my.sharepoint.com/personal/eafrancis_ucsd_edu/Documents/Documents/Rangamani Lab/MATLAB/Muscle calcium model/SkelMuscleCa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46F0245E-E628-4060-900F-B3CF194019C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{46F0245E-E628-4060-900F-B3CF194019C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDE663FE-C4C6-429B-9104-E81B3581445B}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
+    <workbookView xWindow="5670" yWindow="1425" windowWidth="28800" windowHeight="11295" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>A_a</t>
   </si>
@@ -323,10 +323,34 @@
     <t>g_SOCE</t>
   </si>
   <si>
-    <t>B_SRtot</t>
-  </si>
-  <si>
-    <t>K_SRBuffer</t>
+    <t>B_CSQ</t>
+  </si>
+  <si>
+    <t>K_CSQ</t>
+  </si>
+  <si>
+    <t>diffusion_length</t>
+  </si>
+  <si>
+    <t>D_ion</t>
+  </si>
+  <si>
+    <t>D_ATP</t>
+  </si>
+  <si>
+    <t>D_parv</t>
+  </si>
+  <si>
+    <t>D_CSQ</t>
+  </si>
+  <si>
+    <t>D_Pi</t>
+  </si>
+  <si>
+    <t>tau_V</t>
+  </si>
+  <si>
+    <t>k_offCSQ</t>
   </si>
 </sst>
 </file>
@@ -688,16 +712,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -1577,8 +1601,69 @@
         <v>800</v>
       </c>
     </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>104</v>
+      </c>
+      <c r="B98">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>100</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+    </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="5"/>
+      <c r="A103" t="s">
+        <v>101</v>
+      </c>
+      <c r="B103">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>102</v>
+      </c>
+      <c r="B104" s="5">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>103</v>
+      </c>
+      <c r="B105">
+        <v>1.4999999999999999E-4</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E1:G37">
@@ -1590,6 +1675,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001C39BCF8C10C0F4DBE17E99B61C93E7A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3b5ed46e2a2a5b06309d3f0a93e8cdba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xmlns:ns4="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24ef5abf4ddcd47874225b9eda8b4566" ns3:_="" ns4:_="">
     <xsd:import namespace="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
@@ -1778,24 +1880,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FACC7053-B3AF-4F0E-A33A-4CFF5AC23007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05EA78B-E099-49AE-BE0F-B2667B8D5E8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7950FF80-637C-480D-8472-1E87FBE72C09}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1812,29 +1922,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05EA78B-E099-49AE-BE0F-B2667B8D5E8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FACC7053-B3AF-4F0E-A33A-4CFF5AC23007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Set default sodium leak to zero, fix experiment number used to generate uncalibrated plots in SkelMuscleObj. Reorganize TestPlots for clarity.
</commit_message>
<xml_diff>
--- a/InputParam1.xlsx
+++ b/InputParam1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucsdcloud-my.sharepoint.com/personal/eafrancis_ucsd_edu/Documents/Documents/Rangamani Lab/MATLAB/Muscle calcium model/SkelMuscleCa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{46F0245E-E628-4060-900F-B3CF194019C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDE663FE-C4C6-429B-9104-E81B3581445B}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{46F0245E-E628-4060-900F-B3CF194019C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90465DFE-D98A-4FA7-BCED-9CC756B14084}"/>
   <bookViews>
-    <workbookView xWindow="5670" yWindow="1425" windowWidth="28800" windowHeight="11295" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
+    <workbookView xWindow="756" yWindow="0" windowWidth="17652" windowHeight="13680" xr2:uid="{68B96625-8633-4032-98D3-E667FB1B3B8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -413,6 +413,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -714,24 +718,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53993A3-C2AA-418C-9838-9882648AA23B}">
   <dimension ref="A1:F105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E99" sqref="E99"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="47.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="47.33203125" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -741,7 +745,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -751,7 +755,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -761,7 +765,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -771,7 +775,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -781,7 +785,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -791,7 +795,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -801,7 +805,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -811,7 +815,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -821,7 +825,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -831,7 +835,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -841,7 +845,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -851,7 +855,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -861,7 +865,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -871,7 +875,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -881,7 +885,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -891,7 +895,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -901,7 +905,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -911,7 +915,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -921,7 +925,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -931,7 +935,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -941,7 +945,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -951,7 +955,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -961,7 +965,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -971,7 +975,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -981,7 +985,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -991,7 +995,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1001,7 +1005,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -1011,7 +1015,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -1021,7 +1025,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1031,7 +1035,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -1041,7 +1045,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -1051,7 +1055,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -1061,7 +1065,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -1071,7 +1075,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1081,7 +1085,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1091,7 +1095,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -1101,7 +1105,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -1111,7 +1115,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -1121,7 +1125,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>35</v>
       </c>
@@ -1131,7 +1135,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -1141,7 +1145,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1151,7 +1155,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1161,7 +1165,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1171,17 +1175,17 @@
       <c r="E44" s="3"/>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
       <c r="B45">
-        <v>2E-3</v>
+        <v>0</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -1189,7 +1193,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -1197,7 +1201,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -1205,7 +1209,7 @@
         <v>41.7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -1213,7 +1217,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -1221,7 +1225,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -1229,7 +1233,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -1237,7 +1241,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>45</v>
       </c>
@@ -1245,7 +1249,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -1253,7 +1257,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>47</v>
       </c>
@@ -1261,7 +1265,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -1269,7 +1273,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -1277,7 +1281,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>67</v>
       </c>
@@ -1285,7 +1289,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>90</v>
       </c>
@@ -1293,7 +1297,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>91</v>
       </c>
@@ -1301,7 +1305,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>49</v>
       </c>
@@ -1309,7 +1313,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>50</v>
       </c>
@@ -1317,7 +1321,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>51</v>
       </c>
@@ -1326,7 +1330,7 @@
       </c>
       <c r="E63" s="2"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -1334,7 +1338,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>52</v>
       </c>
@@ -1342,7 +1346,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>53</v>
       </c>
@@ -1350,7 +1354,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>54</v>
       </c>
@@ -1358,7 +1362,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>55</v>
       </c>
@@ -1366,7 +1370,7 @@
         <v>6000000</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>56</v>
       </c>
@@ -1374,7 +1378,7 @@
         <v>3.62E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>57</v>
       </c>
@@ -1382,7 +1386,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>58</v>
       </c>
@@ -1391,7 +1395,7 @@
       </c>
       <c r="C71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>59</v>
       </c>
@@ -1399,7 +1403,7 @@
         <v>2.8670000000000001E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -1407,7 +1411,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -1416,7 +1420,7 @@
       </c>
       <c r="D74" s="4"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -1424,7 +1428,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -1432,7 +1436,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -1440,7 +1444,7 @@
         <v>-45</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>75</v>
       </c>
@@ -1448,7 +1452,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -1456,7 +1460,7 @@
         <v>-46</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -1464,7 +1468,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -1472,7 +1476,7 @@
         <v>-78</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -1480,7 +1484,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>80</v>
       </c>
@@ -1488,7 +1492,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>81</v>
       </c>
@@ -1496,7 +1500,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>82</v>
       </c>
@@ -1504,7 +1508,7 @@
         <v>12290</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>83</v>
       </c>
@@ -1512,7 +1516,7 @@
         <v>87500</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>84</v>
       </c>
@@ -1520,7 +1524,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>89</v>
       </c>
@@ -1528,7 +1532,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>85</v>
       </c>
@@ -1536,7 +1540,7 @@
         <v>9.9999999999999991E-6</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>86</v>
       </c>
@@ -1544,7 +1548,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>87</v>
       </c>
@@ -1552,7 +1556,7 @@
         <v>9.3900000000000011E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>88</v>
       </c>
@@ -1560,7 +1564,7 @@
         <v>43846000</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -1568,7 +1572,7 @@
         <v>88.5</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -1576,7 +1580,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -1584,7 +1588,7 @@
         <v>4.7519482988025094E-5</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -1593,7 +1597,7 @@
       </c>
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -1601,7 +1605,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>104</v>
       </c>
@@ -1609,7 +1613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -1617,7 +1621,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -1625,7 +1629,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -1633,7 +1637,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>100</v>
       </c>
@@ -1641,7 +1645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -1649,7 +1653,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -1657,7 +1661,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>103</v>
       </c>
@@ -1675,23 +1679,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001C39BCF8C10C0F4DBE17E99B61C93E7A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3b5ed46e2a2a5b06309d3f0a93e8cdba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xmlns:ns4="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24ef5abf4ddcd47874225b9eda8b4566" ns3:_="" ns4:_="">
     <xsd:import namespace="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
@@ -1880,32 +1867,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FACC7053-B3AF-4F0E-A33A-4CFF5AC23007}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05EA78B-E099-49AE-BE0F-B2667B8D5E8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7950FF80-637C-480D-8472-1E87FBE72C09}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1922,4 +1901,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E05EA78B-E099-49AE-BE0F-B2667B8D5E8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FACC7053-B3AF-4F0E-A33A-4CFF5AC23007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="39c4a7ff-ac0c-43ae-af92-5dd144f40fa2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b007c6b8-87a0-4d8b-8ecf-e3ec3909a945"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>